<commit_message>
Correccion de error en subida por lote
</commit_message>
<xml_diff>
--- a/dist/assets/archivo.xlsx
+++ b/dist/assets/archivo.xlsx
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
-  <si>
-    <t>status_pef</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="77">
   <si>
     <t>id_peso_envio</t>
   </si>
@@ -443,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,18 +456,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -814,7 +799,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -838,16 +823,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -856,89 +841,89 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -948,25 +933,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1504,103 +1483,87 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A1" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="21.875" customWidth="1"/>
-    <col min="3" max="3" width="38.8125" customWidth="1"/>
-    <col min="4" max="4" width="9.125" customWidth="1"/>
-    <col min="5" max="5" width="31.6875" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="38.8125" customWidth="1"/>
+    <col min="3" max="3" width="9.125" customWidth="1"/>
+    <col min="4" max="4" width="31.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26" spans="1:5">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="26" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+    </row>
+    <row r="2" ht="26" spans="1:4">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" ht="26" spans="1:5">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" ht="26" spans="1:4">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
-        <v>100</v>
-      </c>
-      <c r="E2" s="9">
+      <c r="C3" s="3">
+        <v>200</v>
+      </c>
+      <c r="D3" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="26" spans="1:5">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
+    <row r="4" ht="26" spans="1:4">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>300</v>
+      </c>
+      <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4">
-        <v>200</v>
-      </c>
-      <c r="E3" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" ht="26" spans="1:5">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    </row>
+    <row r="5" ht="26" spans="1:4">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4">
-        <v>300</v>
-      </c>
-      <c r="E4" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" ht="26" spans="1:5">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5" s="3">
         <v>150</v>
       </c>
-      <c r="E5" s="9">
+      <c r="D5" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1623,504 +1586,504 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="26" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="14.1875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="48.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.1875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="48.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>21</v>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>27</v>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>29</v>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>30</v>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>31</v>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>32</v>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>33</v>
+      <c r="B24" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>34</v>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>35</v>
+      <c r="B26" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>36</v>
+      <c r="B27" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>37</v>
+      <c r="B28" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>38</v>
+      <c r="B29" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>39</v>
+      <c r="B30" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>40</v>
+      <c r="B31" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>41</v>
+      <c r="B32" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>42</v>
+      <c r="B33" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>43</v>
+      <c r="B34" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>44</v>
+      <c r="B35" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>45</v>
+      <c r="B36" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>46</v>
+      <c r="B37" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>47</v>
+      <c r="B38" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>48</v>
+      <c r="B39" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>49</v>
+      <c r="B40" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>50</v>
+      <c r="B41" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>51</v>
+      <c r="B42" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>52</v>
+      <c r="B43" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>53</v>
+      <c r="B44" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>54</v>
+      <c r="B45" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>55</v>
+      <c r="B46" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>56</v>
+      <c r="B47" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>57</v>
+      <c r="B48" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>58</v>
+      <c r="B49" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>59</v>
+      <c r="B50" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>60</v>
+      <c r="B51" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>61</v>
+      <c r="B52" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>62</v>
+      <c r="B53" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>63</v>
+      <c r="B54" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>64</v>
+      <c r="B55" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>65</v>
+      <c r="B56" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>66</v>
+      <c r="B57" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>67</v>
+      <c r="B58" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>68</v>
+      <c r="B59" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>69</v>
+      <c r="B60" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>70</v>
+      <c r="B61" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>71</v>
+      <c r="B62" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2147,58 +2110,58 @@
   <sheetData>
     <row r="1" ht="26" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" ht="26" spans="1:2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>72</v>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" ht="26" spans="1:2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>73</v>
+      <c r="B3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" ht="26" spans="1:2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>74</v>
+      <c r="B4" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" ht="26" spans="1:2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>75</v>
+      <c r="B5" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="26" spans="1:2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>76</v>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" ht="26" spans="1:2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>77</v>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>